<commit_message>
Fixed IRPStudent.xlsx because it was the wrong format and contained additional fields that are supposed to go into the accommodations file. Added the Designated Supports and Accommodations Excel file which includes accommodations for a single student.
</commit_message>
<xml_diff>
--- a/irp-webapp/src/main/resources/irp-package/IRPStudents.xlsx
+++ b/irp-webapp/src/main/resources/irp-package/IRPStudents.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-140" yWindow="4800" windowWidth="35900" windowHeight="18640" tabRatio="500"/>
+    <workbookView xWindow="40" yWindow="0" windowWidth="38360" windowHeight="8440" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="STUDENT" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="42">
   <si>
     <t>SSID</t>
   </si>
@@ -36,129 +36,6 @@
     <t>CA</t>
   </si>
   <si>
-    <t>State Abbreviation</t>
-  </si>
-  <si>
-    <t>Responsible District Identifier</t>
-  </si>
-  <si>
-    <t>Responsible Institution Identifier</t>
-  </si>
-  <si>
-    <t>Last Or Surname</t>
-  </si>
-  <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Middle Name</t>
-  </si>
-  <si>
-    <t>Birth Date</t>
-  </si>
-  <si>
-    <t>Alternate SSID</t>
-  </si>
-  <si>
-    <t>Grade Level When Assessed</t>
-  </si>
-  <si>
-    <t>Hispanic Or Latino Ethnicity</t>
-  </si>
-  <si>
-    <t>American Indian Or Alaska Native</t>
-  </si>
-  <si>
-    <t>Black Or African American</t>
-  </si>
-  <si>
-    <t>Native Hawaiian Or Other Pacific Islander</t>
-  </si>
-  <si>
-    <t>Demographic Race Two Or More Races</t>
-  </si>
-  <si>
-    <t>IDEA Indicator</t>
-  </si>
-  <si>
-    <t>LEP Status</t>
-  </si>
-  <si>
-    <t>Section 504 Status</t>
-  </si>
-  <si>
-    <t>Economic Disadvantage Status</t>
-  </si>
-  <si>
-    <t>Language Code</t>
-  </si>
-  <si>
-    <t>English Language Proficiency Level</t>
-  </si>
-  <si>
-    <t>Migrant Status</t>
-  </si>
-  <si>
-    <t>First Entry Date Into US School</t>
-  </si>
-  <si>
-    <t>Limited English Proficiency Entry Date</t>
-  </si>
-  <si>
-    <t>LEP Exit Date</t>
-  </si>
-  <si>
-    <t>Title III Language Instruction Program Type</t>
-  </si>
-  <si>
-    <t>Primary Disability Type</t>
-  </si>
-  <si>
-    <t>Subject</t>
-  </si>
-  <si>
-    <t>American Sign Language</t>
-  </si>
-  <si>
-    <t>Color Contrast</t>
-  </si>
-  <si>
-    <t>Closed Captioning</t>
-  </si>
-  <si>
-    <t>Language</t>
-  </si>
-  <si>
-    <t>Masking</t>
-  </si>
-  <si>
-    <t>Permissive Mode</t>
-  </si>
-  <si>
-    <t>Print On Demand</t>
-  </si>
-  <si>
-    <t>Print Size</t>
-  </si>
-  <si>
-    <t>Streamlined Interface</t>
-  </si>
-  <si>
-    <t>Text To Speech</t>
-  </si>
-  <si>
-    <t>Translation</t>
-  </si>
-  <si>
-    <t>Non-Embedded Designated Supports</t>
-  </si>
-  <si>
-    <t>Non-Embedded Accommodations</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
     <t>Male</t>
   </si>
   <si>
@@ -178,12 +55,105 @@
   </si>
   <si>
     <t>Middle</t>
+  </si>
+  <si>
+    <t>2013-01-15</t>
+  </si>
+  <si>
+    <t>2012-06-13</t>
+  </si>
+  <si>
+    <t>DUALLANGUAGE</t>
+  </si>
+  <si>
+    <t>StateAbbreviation</t>
+  </si>
+  <si>
+    <t>ResponsibleDistrictIdentifier</t>
+  </si>
+  <si>
+    <t>ResponsibleInstitutionIdentifier</t>
+  </si>
+  <si>
+    <t>LastOrSurname</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>MiddleName</t>
+  </si>
+  <si>
+    <t>Birthdate</t>
+  </si>
+  <si>
+    <t>AlternateSSID</t>
+  </si>
+  <si>
+    <t>GradeLevelWhenAssessed</t>
+  </si>
+  <si>
+    <t>HispanicOrLatinoEthnicity</t>
+  </si>
+  <si>
+    <t>AmericanIndianOrAlaskaNative</t>
+  </si>
+  <si>
+    <t>BlackOrAfricanAmerican</t>
+  </si>
+  <si>
+    <t>NativeHawaiianOrOtherPacificIslander</t>
+  </si>
+  <si>
+    <t>DemographicRaceTwoOrMoreRaces</t>
+  </si>
+  <si>
+    <t>IDEAIndicator</t>
+  </si>
+  <si>
+    <t>LEPStatus</t>
+  </si>
+  <si>
+    <t>Section504Status</t>
+  </si>
+  <si>
+    <t>EconomicDisadvantageStatus</t>
+  </si>
+  <si>
+    <t>LanguageCode</t>
+  </si>
+  <si>
+    <t>EnglishLanguageProficiencyLevel</t>
+  </si>
+  <si>
+    <t>MigrantStatus</t>
+  </si>
+  <si>
+    <t>FirstEntryDateIntoUSSchool</t>
+  </si>
+  <si>
+    <t>LimitedEnglishProficiencyEntryDate</t>
+  </si>
+  <si>
+    <t>LEPExitDate</t>
+  </si>
+  <si>
+    <t>TitleIIILanguageInstructionProgramType</t>
+  </si>
+  <si>
+    <t>PrimaryDisabilityType</t>
+  </si>
+  <si>
+    <t>Delete</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -230,7 +200,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -256,13 +226,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="25">
+  <cellStyles count="31">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -275,6 +254,9 @@
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -287,6 +269,9 @@
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -616,155 +601,119 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AS13"/>
+  <dimension ref="A1:AE13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="AB8" sqref="AB8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45">
-      <c r="A1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="1" t="s">
+    <row r="1" spans="1:31">
+      <c r="A1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="I1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="P1" s="1" t="s">
+      <c r="O1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA1" s="1" t="s">
+      <c r="Q1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="R1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="S1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="T1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="U1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="V1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="W1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="X1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="Y1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="Z1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AA1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AB1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AC1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AD1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AE1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AP1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>45</v>
-      </c>
     </row>
-    <row r="2" spans="1:45">
+    <row r="2" spans="1:31">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -778,13 +727,13 @@
         <v>39990001</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G2" s="2">
-        <v>39575</v>
+        <v>11</v>
+      </c>
+      <c r="G2" s="4">
+        <v>39508</v>
       </c>
       <c r="H2" s="1">
         <v>39990001</v>
@@ -796,72 +745,60 @@
         <v>3</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="X2" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="X2" s="1">
+        <v>3</v>
+      </c>
       <c r="Y2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="Z2" s="2">
-        <v>42262</v>
+        <v>7</v>
+      </c>
+      <c r="Z2" s="5">
+        <v>40271</v>
       </c>
       <c r="AA2" s="1"/>
       <c r="AB2" s="1"/>
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
       <c r="AE2" s="1"/>
-      <c r="AF2" s="1"/>
-      <c r="AG2" s="1"/>
-      <c r="AH2" s="1"/>
-      <c r="AI2" s="1"/>
-      <c r="AJ2" s="1"/>
-      <c r="AK2" s="1"/>
-      <c r="AL2" s="1"/>
-      <c r="AM2" s="1"/>
-      <c r="AN2" s="1"/>
-      <c r="AO2" s="1"/>
-      <c r="AP2" s="1"/>
-      <c r="AQ2" s="1"/>
-      <c r="AR2" s="1"/>
-      <c r="AS2" s="1"/>
     </row>
-    <row r="3" spans="1:45">
+    <row r="3" spans="1:31">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -875,10 +812,12 @@
         <v>39990002</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="G3" s="4">
+        <v>39509</v>
+      </c>
       <c r="H3" s="1">
         <v>39990002</v>
       </c>
@@ -889,68 +828,60 @@
         <v>3</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X3" s="1">
+        <v>3</v>
+      </c>
       <c r="Y3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="Z3" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="Z3" s="5">
+        <v>40272</v>
+      </c>
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
       <c r="AE3" s="1"/>
-      <c r="AF3" s="1"/>
-      <c r="AG3" s="1"/>
-      <c r="AH3" s="1"/>
-      <c r="AI3" s="1"/>
-      <c r="AJ3" s="1"/>
-      <c r="AK3" s="1"/>
-      <c r="AL3" s="1"/>
-      <c r="AM3" s="1"/>
-      <c r="AN3" s="1"/>
-      <c r="AO3" s="1"/>
-      <c r="AP3" s="1"/>
-      <c r="AQ3" s="1"/>
-      <c r="AR3" s="1"/>
-      <c r="AS3" s="1"/>
     </row>
-    <row r="4" spans="1:45">
+    <row r="4" spans="1:31">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -964,10 +895,12 @@
         <v>39990003</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="G4" s="4">
+        <v>39510</v>
+      </c>
       <c r="H4" s="1">
         <v>39990003</v>
       </c>
@@ -978,68 +911,60 @@
         <v>3</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>51</v>
+        <v>10</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="W4" s="1"/>
-      <c r="X4" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X4" s="1">
+        <v>3</v>
+      </c>
       <c r="Y4" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="Z4" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="Z4" s="5">
+        <v>40273</v>
+      </c>
       <c r="AA4" s="1"/>
       <c r="AB4" s="1"/>
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
       <c r="AE4" s="1"/>
-      <c r="AF4" s="1"/>
-      <c r="AG4" s="1"/>
-      <c r="AH4" s="1"/>
-      <c r="AI4" s="1"/>
-      <c r="AJ4" s="1"/>
-      <c r="AK4" s="1"/>
-      <c r="AL4" s="1"/>
-      <c r="AM4" s="1"/>
-      <c r="AN4" s="1"/>
-      <c r="AO4" s="1"/>
-      <c r="AP4" s="1"/>
-      <c r="AQ4" s="1"/>
-      <c r="AR4" s="1"/>
-      <c r="AS4" s="1"/>
     </row>
-    <row r="5" spans="1:45">
+    <row r="5" spans="1:31">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1053,10 +978,12 @@
         <v>39990004</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="G5" s="4">
+        <v>39511</v>
+      </c>
       <c r="H5" s="1">
         <v>39990004</v>
       </c>
@@ -1067,68 +994,64 @@
         <v>3</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>51</v>
+        <v>10</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="W5" s="1"/>
-      <c r="X5" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X5" s="1">
+        <v>3</v>
+      </c>
       <c r="Y5" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="Z5" s="1"/>
-      <c r="AA5" s="1"/>
-      <c r="AB5" s="1"/>
-      <c r="AC5" s="1"/>
-      <c r="AD5" s="1"/>
-      <c r="AE5" s="1"/>
-      <c r="AF5" s="1"/>
-      <c r="AG5" s="1"/>
-      <c r="AH5" s="1"/>
-      <c r="AI5" s="1"/>
-      <c r="AJ5" s="1"/>
-      <c r="AK5" s="1"/>
-      <c r="AL5" s="1"/>
-      <c r="AM5" s="1"/>
-      <c r="AN5" s="1"/>
-      <c r="AO5" s="1"/>
-      <c r="AP5" s="1"/>
-      <c r="AQ5" s="1"/>
-      <c r="AR5" s="1"/>
-      <c r="AS5" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="Z5" s="5">
+        <v>40274</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="6" spans="1:45">
+    <row r="6" spans="1:31">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1142,11 +1065,11 @@
         <v>79990001</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="F6" s="1"/>
-      <c r="G6" s="2">
-        <v>38629</v>
+      <c r="G6" s="4">
+        <v>38169</v>
       </c>
       <c r="H6" s="1">
         <v>79990001</v>
@@ -1158,68 +1081,58 @@
         <v>7</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="W6" s="1"/>
-      <c r="X6" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X6" s="1">
+        <v>7</v>
+      </c>
       <c r="Y6" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="Z6" s="1"/>
-      <c r="AA6" s="1"/>
+      <c r="AA6" s="2"/>
       <c r="AB6" s="1"/>
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
       <c r="AE6" s="1"/>
-      <c r="AF6" s="1"/>
-      <c r="AG6" s="1"/>
-      <c r="AH6" s="1"/>
-      <c r="AI6" s="1"/>
-      <c r="AJ6" s="1"/>
-      <c r="AK6" s="1"/>
-      <c r="AL6" s="1"/>
-      <c r="AM6" s="1"/>
-      <c r="AN6" s="1"/>
-      <c r="AO6" s="1"/>
-      <c r="AP6" s="1"/>
-      <c r="AQ6" s="1"/>
-      <c r="AR6" s="1"/>
-      <c r="AS6" s="1"/>
     </row>
-    <row r="7" spans="1:45">
+    <row r="7" spans="1:31">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -1233,12 +1146,14 @@
         <v>79990002</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G7" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="G7" s="4">
+        <v>38170</v>
+      </c>
       <c r="H7" s="1">
         <v>79990002</v>
       </c>
@@ -1249,45 +1164,49 @@
         <v>7</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>51</v>
+        <v>10</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="V7" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="W7" s="1"/>
-      <c r="X7" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X7" s="1">
+        <v>7</v>
+      </c>
       <c r="Y7" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
@@ -1295,22 +1214,8 @@
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
       <c r="AE7" s="1"/>
-      <c r="AF7" s="1"/>
-      <c r="AG7" s="1"/>
-      <c r="AH7" s="1"/>
-      <c r="AI7" s="1"/>
-      <c r="AJ7" s="1"/>
-      <c r="AK7" s="1"/>
-      <c r="AL7" s="1"/>
-      <c r="AM7" s="1"/>
-      <c r="AN7" s="1"/>
-      <c r="AO7" s="1"/>
-      <c r="AP7" s="1"/>
-      <c r="AQ7" s="1"/>
-      <c r="AR7" s="1"/>
-      <c r="AS7" s="1"/>
     </row>
-    <row r="8" spans="1:45">
+    <row r="8" spans="1:31">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -1324,10 +1229,12 @@
         <v>79990003</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="G8" s="4">
+        <v>38171</v>
+      </c>
       <c r="H8" s="1">
         <v>79990003</v>
       </c>
@@ -1338,45 +1245,49 @@
         <v>7</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="V8" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="W8" s="1"/>
-      <c r="X8" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X8" s="1">
+        <v>7</v>
+      </c>
       <c r="Y8" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="Z8" s="1"/>
       <c r="AA8" s="1"/>
@@ -1384,22 +1295,8 @@
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
       <c r="AE8" s="1"/>
-      <c r="AF8" s="1"/>
-      <c r="AG8" s="1"/>
-      <c r="AH8" s="1"/>
-      <c r="AI8" s="1"/>
-      <c r="AJ8" s="1"/>
-      <c r="AK8" s="1"/>
-      <c r="AL8" s="1"/>
-      <c r="AM8" s="1"/>
-      <c r="AN8" s="1"/>
-      <c r="AO8" s="1"/>
-      <c r="AP8" s="1"/>
-      <c r="AQ8" s="1"/>
-      <c r="AR8" s="1"/>
-      <c r="AS8" s="1"/>
     </row>
-    <row r="9" spans="1:45">
+    <row r="9" spans="1:31">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -1413,10 +1310,12 @@
         <v>79990004</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="G9" s="4">
+        <v>38172</v>
+      </c>
       <c r="H9" s="1">
         <v>79990004</v>
       </c>
@@ -1427,45 +1326,49 @@
         <v>7</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="S9" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="V9" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="W9" s="1"/>
-      <c r="X9" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X9" s="1">
+        <v>7</v>
+      </c>
       <c r="Y9" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="Z9" s="1"/>
       <c r="AA9" s="1"/>
@@ -1473,22 +1376,8 @@
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
       <c r="AE9" s="1"/>
-      <c r="AF9" s="1"/>
-      <c r="AG9" s="1"/>
-      <c r="AH9" s="1"/>
-      <c r="AI9" s="1"/>
-      <c r="AJ9" s="1"/>
-      <c r="AK9" s="1"/>
-      <c r="AL9" s="1"/>
-      <c r="AM9" s="1"/>
-      <c r="AN9" s="1"/>
-      <c r="AO9" s="1"/>
-      <c r="AP9" s="1"/>
-      <c r="AQ9" s="1"/>
-      <c r="AR9" s="1"/>
-      <c r="AS9" s="1"/>
     </row>
-    <row r="10" spans="1:45">
+    <row r="10" spans="1:31">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
@@ -1502,12 +1391,14 @@
         <v>119990001</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G10" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="G10" s="4">
+        <v>35735</v>
+      </c>
       <c r="H10" s="1">
         <v>119990001</v>
       </c>
@@ -1518,45 +1409,49 @@
         <v>11</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="V10" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="W10" s="1"/>
-      <c r="X10" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X10" s="1">
+        <v>11</v>
+      </c>
       <c r="Y10" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
@@ -1564,22 +1459,8 @@
       <c r="AC10" s="1"/>
       <c r="AD10" s="1"/>
       <c r="AE10" s="1"/>
-      <c r="AF10" s="1"/>
-      <c r="AG10" s="1"/>
-      <c r="AH10" s="1"/>
-      <c r="AI10" s="1"/>
-      <c r="AJ10" s="1"/>
-      <c r="AK10" s="1"/>
-      <c r="AL10" s="1"/>
-      <c r="AM10" s="1"/>
-      <c r="AN10" s="1"/>
-      <c r="AO10" s="1"/>
-      <c r="AP10" s="1"/>
-      <c r="AQ10" s="1"/>
-      <c r="AR10" s="1"/>
-      <c r="AS10" s="1"/>
     </row>
-    <row r="11" spans="1:45">
+    <row r="11" spans="1:31">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
@@ -1593,10 +1474,12 @@
         <v>119990002</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="G11" s="4">
+        <v>35736</v>
+      </c>
       <c r="H11" s="1">
         <v>119990002</v>
       </c>
@@ -1607,45 +1490,49 @@
         <v>11</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="U11" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="V11" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="W11" s="1"/>
-      <c r="X11" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="W11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X11" s="1">
+        <v>11</v>
+      </c>
       <c r="Y11" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
@@ -1653,22 +1540,8 @@
       <c r="AC11" s="1"/>
       <c r="AD11" s="1"/>
       <c r="AE11" s="1"/>
-      <c r="AF11" s="1"/>
-      <c r="AG11" s="1"/>
-      <c r="AH11" s="1"/>
-      <c r="AI11" s="1"/>
-      <c r="AJ11" s="1"/>
-      <c r="AK11" s="1"/>
-      <c r="AL11" s="1"/>
-      <c r="AM11" s="1"/>
-      <c r="AN11" s="1"/>
-      <c r="AO11" s="1"/>
-      <c r="AP11" s="1"/>
-      <c r="AQ11" s="1"/>
-      <c r="AR11" s="1"/>
-      <c r="AS11" s="1"/>
     </row>
-    <row r="12" spans="1:45">
+    <row r="12" spans="1:31">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
@@ -1682,10 +1555,12 @@
         <v>119990004</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="G12" s="4">
+        <v>35737</v>
+      </c>
       <c r="H12" s="1">
         <v>119990004</v>
       </c>
@@ -1696,45 +1571,49 @@
         <v>11</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="V12" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="W12" s="1"/>
-      <c r="X12" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="W12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X12" s="1">
+        <v>11</v>
+      </c>
       <c r="Y12" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
@@ -1742,22 +1621,8 @@
       <c r="AC12" s="1"/>
       <c r="AD12" s="1"/>
       <c r="AE12" s="1"/>
-      <c r="AF12" s="1"/>
-      <c r="AG12" s="1"/>
-      <c r="AH12" s="1"/>
-      <c r="AI12" s="1"/>
-      <c r="AJ12" s="1"/>
-      <c r="AK12" s="1"/>
-      <c r="AL12" s="1"/>
-      <c r="AM12" s="1"/>
-      <c r="AN12" s="1"/>
-      <c r="AO12" s="1"/>
-      <c r="AP12" s="1"/>
-      <c r="AQ12" s="1"/>
-      <c r="AR12" s="1"/>
-      <c r="AS12" s="1"/>
     </row>
-    <row r="13" spans="1:45">
+    <row r="13" spans="1:31">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
@@ -1771,10 +1636,12 @@
         <v>119990005</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="G13" s="4">
+        <v>35738</v>
+      </c>
       <c r="H13" s="1">
         <v>119990005</v>
       </c>
@@ -1785,45 +1652,49 @@
         <v>11</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="S13" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="U13" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="V13" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="W13" s="1"/>
-      <c r="X13" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="W13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X13" s="1">
+        <v>11</v>
+      </c>
       <c r="Y13" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="Z13" s="1"/>
       <c r="AA13" s="1"/>
@@ -1831,20 +1702,6 @@
       <c r="AC13" s="1"/>
       <c r="AD13" s="1"/>
       <c r="AE13" s="1"/>
-      <c r="AF13" s="1"/>
-      <c r="AG13" s="1"/>
-      <c r="AH13" s="1"/>
-      <c r="AI13" s="1"/>
-      <c r="AJ13" s="1"/>
-      <c r="AK13" s="1"/>
-      <c r="AL13" s="1"/>
-      <c r="AM13" s="1"/>
-      <c r="AN13" s="1"/>
-      <c r="AO13" s="1"/>
-      <c r="AP13" s="1"/>
-      <c r="AQ13" s="1"/>
-      <c r="AR13" s="1"/>
-      <c r="AS13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Updated IRP Student file includes more students
</commit_message>
<xml_diff>
--- a/irp-webapp/src/main/resources/irp-package/IRPStudents.xlsx
+++ b/irp-webapp/src/main/resources/irp-package/IRPStudents.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="0" windowWidth="38360" windowHeight="8440" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="23460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="STUDENT" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="157">
   <si>
     <t>SSID</t>
   </si>
@@ -48,15 +48,9 @@
     <t>eng</t>
   </si>
   <si>
-    <t>Student</t>
-  </si>
-  <si>
     <t>Female</t>
   </si>
   <si>
-    <t>Middle</t>
-  </si>
-  <si>
     <t>2013-01-15</t>
   </si>
   <si>
@@ -145,6 +139,357 @@
   </si>
   <si>
     <t>Delete</t>
+  </si>
+  <si>
+    <t>StudentA</t>
+  </si>
+  <si>
+    <t>StudentB</t>
+  </si>
+  <si>
+    <t>StudentC</t>
+  </si>
+  <si>
+    <t>StudentD</t>
+  </si>
+  <si>
+    <t>LastNameA</t>
+  </si>
+  <si>
+    <t>LastNameB</t>
+  </si>
+  <si>
+    <t>LastNameC</t>
+  </si>
+  <si>
+    <t>LastNameD</t>
+  </si>
+  <si>
+    <t>LastNameE</t>
+  </si>
+  <si>
+    <t>LastNameF</t>
+  </si>
+  <si>
+    <t>LastNameG</t>
+  </si>
+  <si>
+    <t>LastNameH</t>
+  </si>
+  <si>
+    <t>LastNameI</t>
+  </si>
+  <si>
+    <t>LastNameJ</t>
+  </si>
+  <si>
+    <t>LastNameK</t>
+  </si>
+  <si>
+    <t>LastNameL</t>
+  </si>
+  <si>
+    <t>StudentE</t>
+  </si>
+  <si>
+    <t>StudentF</t>
+  </si>
+  <si>
+    <t>StudentG</t>
+  </si>
+  <si>
+    <t>StudentH</t>
+  </si>
+  <si>
+    <t>StudentI</t>
+  </si>
+  <si>
+    <t>StudentJ</t>
+  </si>
+  <si>
+    <t>StudentK</t>
+  </si>
+  <si>
+    <t>StudentL</t>
+  </si>
+  <si>
+    <t>LastNameM</t>
+  </si>
+  <si>
+    <t>LastNameN</t>
+  </si>
+  <si>
+    <t>LastNameO</t>
+  </si>
+  <si>
+    <t>LastNameP</t>
+  </si>
+  <si>
+    <t>LastNameQ</t>
+  </si>
+  <si>
+    <t>LastNameR</t>
+  </si>
+  <si>
+    <t>LastNameS</t>
+  </si>
+  <si>
+    <t>LastNameT</t>
+  </si>
+  <si>
+    <t>LastNameU</t>
+  </si>
+  <si>
+    <t>LastNameV</t>
+  </si>
+  <si>
+    <t>LastNameW</t>
+  </si>
+  <si>
+    <t>LastNameX</t>
+  </si>
+  <si>
+    <t>StudentM</t>
+  </si>
+  <si>
+    <t>StudentN</t>
+  </si>
+  <si>
+    <t>StudentO</t>
+  </si>
+  <si>
+    <t>StudentP</t>
+  </si>
+  <si>
+    <t>StudentQ</t>
+  </si>
+  <si>
+    <t>StudentR</t>
+  </si>
+  <si>
+    <t>StudentS</t>
+  </si>
+  <si>
+    <t>StudentT</t>
+  </si>
+  <si>
+    <t>StudentU</t>
+  </si>
+  <si>
+    <t>StudentV</t>
+  </si>
+  <si>
+    <t>StudentW</t>
+  </si>
+  <si>
+    <t>StudentX</t>
+  </si>
+  <si>
+    <t>LastNameY</t>
+  </si>
+  <si>
+    <t>LastNameZ</t>
+  </si>
+  <si>
+    <t>LastNameAA</t>
+  </si>
+  <si>
+    <t>LastNameAB</t>
+  </si>
+  <si>
+    <t>LastNameAC</t>
+  </si>
+  <si>
+    <t>LastNameAD</t>
+  </si>
+  <si>
+    <t>LastNameAE</t>
+  </si>
+  <si>
+    <t>LastNameAF</t>
+  </si>
+  <si>
+    <t>LastNameAG</t>
+  </si>
+  <si>
+    <t>LastNameAH</t>
+  </si>
+  <si>
+    <t>LastNameAI</t>
+  </si>
+  <si>
+    <t>LastNameAJ</t>
+  </si>
+  <si>
+    <t>StudentY</t>
+  </si>
+  <si>
+    <t>StudentZ</t>
+  </si>
+  <si>
+    <t>StudentAA</t>
+  </si>
+  <si>
+    <t>StudentAB</t>
+  </si>
+  <si>
+    <t>StudentAC</t>
+  </si>
+  <si>
+    <t>StudentAD</t>
+  </si>
+  <si>
+    <t>StudentAE</t>
+  </si>
+  <si>
+    <t>StudentAF</t>
+  </si>
+  <si>
+    <t>StudentAG</t>
+  </si>
+  <si>
+    <t>StudentAH</t>
+  </si>
+  <si>
+    <t>StudentAI</t>
+  </si>
+  <si>
+    <t>StudentAJ</t>
+  </si>
+  <si>
+    <t>A39990001</t>
+  </si>
+  <si>
+    <t>A39990002</t>
+  </si>
+  <si>
+    <t>A39990003</t>
+  </si>
+  <si>
+    <t>A39990004</t>
+  </si>
+  <si>
+    <t>A39990005</t>
+  </si>
+  <si>
+    <t>A39990006</t>
+  </si>
+  <si>
+    <t>A39990007</t>
+  </si>
+  <si>
+    <t>A39990008</t>
+  </si>
+  <si>
+    <t>A39990009</t>
+  </si>
+  <si>
+    <t>A39990010</t>
+  </si>
+  <si>
+    <t>A39990011</t>
+  </si>
+  <si>
+    <t>A39990012</t>
+  </si>
+  <si>
+    <t>A79990001</t>
+  </si>
+  <si>
+    <t>A79990002</t>
+  </si>
+  <si>
+    <t>A79990003</t>
+  </si>
+  <si>
+    <t>A79990004</t>
+  </si>
+  <si>
+    <t>A79990005</t>
+  </si>
+  <si>
+    <t>A79990006</t>
+  </si>
+  <si>
+    <t>A79990007</t>
+  </si>
+  <si>
+    <t>A79990008</t>
+  </si>
+  <si>
+    <t>A79990009</t>
+  </si>
+  <si>
+    <t>A79990010</t>
+  </si>
+  <si>
+    <t>A79990011</t>
+  </si>
+  <si>
+    <t>A79990012</t>
+  </si>
+  <si>
+    <t>A119990001</t>
+  </si>
+  <si>
+    <t>A119990002</t>
+  </si>
+  <si>
+    <t>A119990003</t>
+  </si>
+  <si>
+    <t>A119990004</t>
+  </si>
+  <si>
+    <t>A119990005</t>
+  </si>
+  <si>
+    <t>A119990006</t>
+  </si>
+  <si>
+    <t>A119990007</t>
+  </si>
+  <si>
+    <t>A119990008</t>
+  </si>
+  <si>
+    <t>A119990009</t>
+  </si>
+  <si>
+    <t>A119990010</t>
+  </si>
+  <si>
+    <t>A119990011</t>
+  </si>
+  <si>
+    <t>A119990012</t>
+  </si>
+  <si>
+    <t>MiddleA</t>
+  </si>
+  <si>
+    <t>MiddleE</t>
+  </si>
+  <si>
+    <t>MiddleI</t>
+  </si>
+  <si>
+    <t>MiddleN</t>
+  </si>
+  <si>
+    <t>MiddleR</t>
+  </si>
+  <si>
+    <t>MiddleV</t>
+  </si>
+  <si>
+    <t>MiddleY</t>
+  </si>
+  <si>
+    <t>MiddleAC</t>
+  </si>
+  <si>
+    <t>MiddleAG</t>
   </si>
 </sst>
 </file>
@@ -152,7 +497,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -200,7 +545,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -232,16 +577,47 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="59">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -257,6 +633,20 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -272,6 +662,20 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -601,10 +1005,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE13"/>
+  <dimension ref="A1:AE37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB8" sqref="AB8"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="AA14" sqref="AA14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -620,97 +1024,97 @@
   <sheetData>
     <row r="1" spans="1:31">
       <c r="A1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="I1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="N1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="Q1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="S1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="AD1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE1" s="3" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:31">
@@ -723,14 +1127,14 @@
       <c r="C2" s="1">
         <v>1</v>
       </c>
-      <c r="D2" s="1">
-        <v>39990001</v>
+      <c r="D2" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>148</v>
       </c>
       <c r="G2" s="4">
         <v>39508</v>
@@ -738,8 +1142,8 @@
       <c r="H2" s="1">
         <v>39990001</v>
       </c>
-      <c r="I2" s="1">
-        <v>39990001</v>
+      <c r="I2" s="6" t="s">
+        <v>112</v>
       </c>
       <c r="J2" s="1">
         <v>3</v>
@@ -790,7 +1194,7 @@
         <v>7</v>
       </c>
       <c r="Z2" s="5">
-        <v>40271</v>
+        <v>40393</v>
       </c>
       <c r="AA2" s="1"/>
       <c r="AB2" s="1"/>
@@ -808,11 +1212,11 @@
       <c r="C3" s="1">
         <v>1</v>
       </c>
-      <c r="D3" s="1">
-        <v>39990002</v>
+      <c r="D3" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="4">
@@ -821,8 +1225,8 @@
       <c r="H3" s="1">
         <v>39990002</v>
       </c>
-      <c r="I3" s="1">
-        <v>39990002</v>
+      <c r="I3" s="6" t="s">
+        <v>113</v>
       </c>
       <c r="J3" s="1">
         <v>3</v>
@@ -873,7 +1277,7 @@
         <v>7</v>
       </c>
       <c r="Z3" s="5">
-        <v>40272</v>
+        <v>40394</v>
       </c>
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
@@ -891,11 +1295,11 @@
       <c r="C4" s="1">
         <v>1</v>
       </c>
-      <c r="D4" s="1">
-        <v>39990003</v>
+      <c r="D4" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="4">
@@ -904,14 +1308,14 @@
       <c r="H4" s="1">
         <v>39990003</v>
       </c>
-      <c r="I4" s="1">
-        <v>39990003</v>
+      <c r="I4" s="6" t="s">
+        <v>114</v>
       </c>
       <c r="J4" s="1">
         <v>3</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>7</v>
@@ -956,7 +1360,7 @@
         <v>7</v>
       </c>
       <c r="Z4" s="5">
-        <v>40273</v>
+        <v>40395</v>
       </c>
       <c r="AA4" s="1"/>
       <c r="AB4" s="1"/>
@@ -974,11 +1378,11 @@
       <c r="C5" s="1">
         <v>1</v>
       </c>
-      <c r="D5" s="1">
-        <v>39990004</v>
+      <c r="D5" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="4">
@@ -987,14 +1391,14 @@
       <c r="H5" s="1">
         <v>39990004</v>
       </c>
-      <c r="I5" s="1">
-        <v>39990004</v>
+      <c r="I5" s="6" t="s">
+        <v>115</v>
       </c>
       <c r="J5" s="1">
         <v>3</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>7</v>
@@ -1039,16 +1443,16 @@
         <v>7</v>
       </c>
       <c r="Z5" s="5">
-        <v>40274</v>
+        <v>40396</v>
       </c>
       <c r="AA5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC5" t="s">
         <v>12</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:31">
@@ -1061,24 +1465,26 @@
       <c r="C6" s="1">
         <v>1</v>
       </c>
-      <c r="D6" s="1">
-        <v>79990001</v>
+      <c r="D6" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="1"/>
+        <v>56</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>149</v>
+      </c>
       <c r="G6" s="4">
-        <v>38169</v>
+        <v>39512</v>
       </c>
       <c r="H6" s="1">
-        <v>79990001</v>
-      </c>
-      <c r="I6" s="1">
-        <v>79990001</v>
+        <v>39990005</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>116</v>
       </c>
       <c r="J6" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>5</v>
@@ -1102,7 +1508,7 @@
         <v>7</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S6" s="1" t="s">
         <v>7</v>
@@ -1120,13 +1526,15 @@
         <v>8</v>
       </c>
       <c r="X6" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="Y6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Z6" s="1"/>
-      <c r="AA6" s="2"/>
+      <c r="Z6" s="5">
+        <v>40397</v>
+      </c>
+      <c r="AA6" s="1"/>
       <c r="AB6" s="1"/>
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
@@ -1142,38 +1550,36 @@
       <c r="C7" s="1">
         <v>1</v>
       </c>
-      <c r="D7" s="1">
-        <v>79990002</v>
+      <c r="D7" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>11</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="F7" s="1"/>
       <c r="G7" s="4">
-        <v>38170</v>
+        <v>39513</v>
       </c>
       <c r="H7" s="1">
-        <v>79990002</v>
-      </c>
-      <c r="I7" s="1">
-        <v>79990002</v>
+        <v>39990006</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>117</v>
       </c>
       <c r="J7" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>7</v>
@@ -1191,7 +1597,7 @@
         <v>7</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="U7" s="1" t="s">
         <v>7</v>
@@ -1203,12 +1609,14 @@
         <v>8</v>
       </c>
       <c r="X7" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="Y7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Z7" s="1"/>
+      <c r="Z7" s="5">
+        <v>40398</v>
+      </c>
       <c r="AA7" s="1"/>
       <c r="AB7" s="1"/>
       <c r="AC7" s="1"/>
@@ -1225,27 +1633,27 @@
       <c r="C8" s="1">
         <v>1</v>
       </c>
-      <c r="D8" s="1">
-        <v>79990003</v>
+      <c r="D8" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="4">
-        <v>38171</v>
+        <v>39514</v>
       </c>
       <c r="H8" s="1">
-        <v>79990003</v>
-      </c>
-      <c r="I8" s="1">
-        <v>79990003</v>
+        <v>39990007</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>118</v>
       </c>
       <c r="J8" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>7</v>
@@ -1254,10 +1662,10 @@
         <v>7</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P8" s="1" t="s">
         <v>7</v>
@@ -1278,18 +1686,20 @@
         <v>7</v>
       </c>
       <c r="V8" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="W8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="X8" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="Y8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Z8" s="1"/>
+      <c r="Z8" s="5">
+        <v>40399</v>
+      </c>
       <c r="AA8" s="1"/>
       <c r="AB8" s="1"/>
       <c r="AC8" s="1"/>
@@ -1306,27 +1716,27 @@
       <c r="C9" s="1">
         <v>1</v>
       </c>
-      <c r="D9" s="1">
-        <v>79990004</v>
+      <c r="D9" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="4">
-        <v>38172</v>
+        <v>39515</v>
       </c>
       <c r="H9" s="1">
-        <v>79990004</v>
-      </c>
-      <c r="I9" s="1">
-        <v>79990004</v>
+        <v>39990008</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>119</v>
       </c>
       <c r="J9" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>7</v>
@@ -1335,13 +1745,13 @@
         <v>7</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q9" s="1" t="s">
         <v>7</v>
@@ -1365,17 +1775,23 @@
         <v>8</v>
       </c>
       <c r="X9" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="Y9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Z9" s="1"/>
-      <c r="AA9" s="1"/>
-      <c r="AB9" s="1"/>
-      <c r="AC9" s="1"/>
-      <c r="AD9" s="1"/>
-      <c r="AE9" s="1"/>
+      <c r="Z9" s="5">
+        <v>40400</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="10" spans="1:31">
       <c r="A10" s="1" t="s">
@@ -1387,38 +1803,38 @@
       <c r="C10" s="1">
         <v>1</v>
       </c>
-      <c r="D10" s="1">
-        <v>119990001</v>
+      <c r="D10" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>9</v>
+        <v>60</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>11</v>
+        <v>150</v>
       </c>
       <c r="G10" s="4">
-        <v>35735</v>
+        <v>39516</v>
       </c>
       <c r="H10" s="1">
-        <v>119990001</v>
-      </c>
-      <c r="I10" s="1">
-        <v>119990001</v>
+        <v>39990009</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>120</v>
       </c>
       <c r="J10" s="1">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>5</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>7</v>
@@ -1433,7 +1849,7 @@
         <v>7</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="T10" s="1" t="s">
         <v>7</v>
@@ -1448,12 +1864,14 @@
         <v>8</v>
       </c>
       <c r="X10" s="1">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="Y10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Z10" s="1"/>
+      <c r="Z10" s="5">
+        <v>40401</v>
+      </c>
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
       <c r="AC10" s="1"/>
@@ -1470,24 +1888,24 @@
       <c r="C11" s="1">
         <v>1</v>
       </c>
-      <c r="D11" s="1">
-        <v>119990002</v>
+      <c r="D11" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="4">
-        <v>35736</v>
+        <v>39517</v>
       </c>
       <c r="H11" s="1">
-        <v>119990002</v>
-      </c>
-      <c r="I11" s="1">
-        <v>119990002</v>
+        <v>39990010</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>121</v>
       </c>
       <c r="J11" s="1">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>5</v>
@@ -1517,7 +1935,7 @@
         <v>7</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="U11" s="1" t="s">
         <v>7</v>
@@ -1529,12 +1947,14 @@
         <v>8</v>
       </c>
       <c r="X11" s="1">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="Y11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Z11" s="1"/>
+      <c r="Z11" s="5">
+        <v>40402</v>
+      </c>
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
       <c r="AC11" s="1"/>
@@ -1551,27 +1971,27 @@
       <c r="C12" s="1">
         <v>1</v>
       </c>
-      <c r="D12" s="1">
-        <v>119990004</v>
+      <c r="D12" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>9</v>
+        <v>62</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="4">
-        <v>35737</v>
+        <v>39518</v>
       </c>
       <c r="H12" s="1">
-        <v>119990004</v>
-      </c>
-      <c r="I12" s="1">
-        <v>119990004</v>
+        <v>39990011</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>122</v>
       </c>
       <c r="J12" s="1">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>7</v>
@@ -1580,10 +2000,10 @@
         <v>7</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P12" s="1" t="s">
         <v>7</v>
@@ -1601,7 +2021,7 @@
         <v>7</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="V12" s="1" t="s">
         <v>7</v>
@@ -1610,12 +2030,14 @@
         <v>8</v>
       </c>
       <c r="X12" s="1">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="Y12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Z12" s="1"/>
+      <c r="Z12" s="5">
+        <v>40403</v>
+      </c>
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
       <c r="AC12" s="1"/>
@@ -1632,27 +2054,27 @@
       <c r="C13" s="1">
         <v>1</v>
       </c>
-      <c r="D13" s="1">
-        <v>119990005</v>
+      <c r="D13" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="4">
-        <v>35738</v>
+        <v>39519</v>
       </c>
       <c r="H13" s="1">
-        <v>119990005</v>
-      </c>
-      <c r="I13" s="1">
-        <v>119990005</v>
+        <v>39990012</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>123</v>
       </c>
       <c r="J13" s="1">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>7</v>
@@ -1667,10 +2089,10 @@
         <v>7</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R13" s="1" t="s">
         <v>7</v>
@@ -1691,17 +2113,2027 @@
         <v>8</v>
       </c>
       <c r="X13" s="1">
+        <v>3</v>
+      </c>
+      <c r="Y13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z13" s="5">
+        <v>40404</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB13" t="s">
         <v>11</v>
       </c>
-      <c r="Y13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Z13" s="1"/>
-      <c r="AA13" s="1"/>
-      <c r="AB13" s="1"/>
-      <c r="AC13" s="1"/>
-      <c r="AD13" s="1"/>
-      <c r="AE13" s="1"/>
+      <c r="AC13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31">
+      <c r="A14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="4">
+        <v>38169</v>
+      </c>
+      <c r="H14" s="1">
+        <v>79990001</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="J14" s="1">
+        <v>7</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="V14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X14" s="1">
+        <v>7</v>
+      </c>
+      <c r="Y14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z14" s="5">
+        <v>38961</v>
+      </c>
+      <c r="AA14" s="2"/>
+      <c r="AB14" s="1"/>
+      <c r="AC14" s="1"/>
+      <c r="AD14" s="1"/>
+      <c r="AE14" s="1"/>
+    </row>
+    <row r="15" spans="1:31">
+      <c r="A15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G15" s="4">
+        <v>38170</v>
+      </c>
+      <c r="H15" s="1">
+        <v>79990002</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J15" s="1">
+        <v>7</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="V15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X15" s="1">
+        <v>7</v>
+      </c>
+      <c r="Y15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z15" s="5">
+        <v>38962</v>
+      </c>
+      <c r="AA15" s="1"/>
+      <c r="AB15" s="1"/>
+      <c r="AC15" s="1"/>
+      <c r="AD15" s="1"/>
+      <c r="AE15" s="1"/>
+    </row>
+    <row r="16" spans="1:31">
+      <c r="A16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="4">
+        <v>38171</v>
+      </c>
+      <c r="H16" s="1">
+        <v>79990003</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="J16" s="1">
+        <v>7</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="V16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="W16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X16" s="1">
+        <v>7</v>
+      </c>
+      <c r="Y16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z16" s="5">
+        <v>38963</v>
+      </c>
+      <c r="AA16" s="1"/>
+      <c r="AB16" s="1"/>
+      <c r="AC16" s="1"/>
+      <c r="AD16" s="1"/>
+      <c r="AE16" s="1"/>
+    </row>
+    <row r="17" spans="1:31">
+      <c r="A17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="4">
+        <v>38172</v>
+      </c>
+      <c r="H17" s="1">
+        <v>79990004</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="J17" s="1">
+        <v>7</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="V17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X17" s="1">
+        <v>7</v>
+      </c>
+      <c r="Y17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z17" s="5">
+        <v>38964</v>
+      </c>
+      <c r="AA17" s="1"/>
+      <c r="AB17" s="1"/>
+      <c r="AC17" s="1"/>
+      <c r="AD17" s="1"/>
+      <c r="AE17" s="1"/>
+    </row>
+    <row r="18" spans="1:31">
+      <c r="A18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F18" s="1"/>
+      <c r="G18" s="4">
+        <v>38173</v>
+      </c>
+      <c r="H18" s="1">
+        <v>79990005</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="J18" s="1">
+        <v>7</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="V18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X18" s="1">
+        <v>7</v>
+      </c>
+      <c r="Y18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z18" s="5">
+        <v>38965</v>
+      </c>
+      <c r="AA18" s="2"/>
+      <c r="AB18" s="1"/>
+      <c r="AC18" s="1"/>
+      <c r="AD18" s="1"/>
+      <c r="AE18" s="1"/>
+    </row>
+    <row r="19" spans="1:31">
+      <c r="A19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="G19" s="4">
+        <v>38174</v>
+      </c>
+      <c r="H19" s="1">
+        <v>79990006</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="J19" s="1">
+        <v>7</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="V19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X19" s="1">
+        <v>7</v>
+      </c>
+      <c r="Y19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z19" s="5">
+        <v>38966</v>
+      </c>
+      <c r="AA19" s="1"/>
+      <c r="AB19" s="1"/>
+      <c r="AC19" s="1"/>
+      <c r="AD19" s="1"/>
+      <c r="AE19" s="1"/>
+    </row>
+    <row r="20" spans="1:31">
+      <c r="A20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="4">
+        <v>38175</v>
+      </c>
+      <c r="H20" s="1">
+        <v>79990007</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="J20" s="1">
+        <v>7</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="V20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="W20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X20" s="1">
+        <v>7</v>
+      </c>
+      <c r="Y20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z20" s="5">
+        <v>38967</v>
+      </c>
+      <c r="AA20" s="1"/>
+      <c r="AB20" s="1"/>
+      <c r="AC20" s="1"/>
+      <c r="AD20" s="1"/>
+      <c r="AE20" s="1"/>
+    </row>
+    <row r="21" spans="1:31">
+      <c r="A21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F21" s="1"/>
+      <c r="G21" s="4">
+        <v>38176</v>
+      </c>
+      <c r="H21" s="1">
+        <v>79990008</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="J21" s="1">
+        <v>7</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="V21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X21" s="1">
+        <v>7</v>
+      </c>
+      <c r="Y21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z21" s="5">
+        <v>38968</v>
+      </c>
+      <c r="AA21" s="1"/>
+      <c r="AB21" s="1"/>
+      <c r="AC21" s="1"/>
+      <c r="AD21" s="1"/>
+      <c r="AE21" s="1"/>
+    </row>
+    <row r="22" spans="1:31">
+      <c r="A22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="4">
+        <v>38177</v>
+      </c>
+      <c r="H22" s="1">
+        <v>79990009</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="J22" s="1">
+        <v>7</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="V22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X22" s="1">
+        <v>7</v>
+      </c>
+      <c r="Y22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z22" s="5">
+        <v>38969</v>
+      </c>
+      <c r="AA22" s="2"/>
+      <c r="AB22" s="1"/>
+      <c r="AC22" s="1"/>
+      <c r="AD22" s="1"/>
+      <c r="AE22" s="1"/>
+    </row>
+    <row r="23" spans="1:31">
+      <c r="A23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G23" s="4">
+        <v>38178</v>
+      </c>
+      <c r="H23" s="1">
+        <v>79990010</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="J23" s="1">
+        <v>7</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="V23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X23" s="1">
+        <v>7</v>
+      </c>
+      <c r="Y23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z23" s="5">
+        <v>38970</v>
+      </c>
+      <c r="AA23" s="1"/>
+      <c r="AB23" s="1"/>
+      <c r="AC23" s="1"/>
+      <c r="AD23" s="1"/>
+      <c r="AE23" s="1"/>
+    </row>
+    <row r="24" spans="1:31">
+      <c r="A24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F24" s="1"/>
+      <c r="G24" s="4">
+        <v>38179</v>
+      </c>
+      <c r="H24" s="1">
+        <v>79990011</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="J24" s="1">
+        <v>7</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="V24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="W24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X24" s="1">
+        <v>7</v>
+      </c>
+      <c r="Y24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z24" s="5">
+        <v>38971</v>
+      </c>
+      <c r="AA24" s="1"/>
+      <c r="AB24" s="1"/>
+      <c r="AC24" s="1"/>
+      <c r="AD24" s="1"/>
+      <c r="AE24" s="1"/>
+    </row>
+    <row r="25" spans="1:31">
+      <c r="A25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F25" s="1"/>
+      <c r="G25" s="4">
+        <v>38180</v>
+      </c>
+      <c r="H25" s="1">
+        <v>79990012</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="J25" s="1">
+        <v>7</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="V25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X25" s="1">
+        <v>7</v>
+      </c>
+      <c r="Y25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z25" s="5">
+        <v>38972</v>
+      </c>
+      <c r="AA25" s="1"/>
+      <c r="AB25" s="1"/>
+      <c r="AC25" s="1"/>
+      <c r="AD25" s="1"/>
+      <c r="AE25" s="1"/>
+    </row>
+    <row r="26" spans="1:31">
+      <c r="A26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G26" s="4">
+        <v>35735</v>
+      </c>
+      <c r="H26" s="1">
+        <v>119990001</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="J26" s="1">
+        <v>11</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="T26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="V26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X26" s="1">
+        <v>11</v>
+      </c>
+      <c r="Y26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z26" s="5">
+        <v>37865</v>
+      </c>
+      <c r="AA26" s="1"/>
+      <c r="AB26" s="1"/>
+      <c r="AC26" s="1"/>
+      <c r="AD26" s="1"/>
+      <c r="AE26" s="1"/>
+    </row>
+    <row r="27" spans="1:31">
+      <c r="A27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
+      <c r="C27" s="1">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F27" s="1"/>
+      <c r="G27" s="4">
+        <v>35736</v>
+      </c>
+      <c r="H27" s="1">
+        <v>119990002</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="J27" s="1">
+        <v>11</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="V27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X27" s="1">
+        <v>11</v>
+      </c>
+      <c r="Y27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z27" s="5">
+        <v>37866</v>
+      </c>
+      <c r="AA27" s="1"/>
+      <c r="AB27" s="1"/>
+      <c r="AC27" s="1"/>
+      <c r="AD27" s="1"/>
+      <c r="AE27" s="1"/>
+    </row>
+    <row r="28" spans="1:31">
+      <c r="A28" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F28" s="1"/>
+      <c r="G28" s="4">
+        <v>35737</v>
+      </c>
+      <c r="H28" s="1">
+        <v>119990003</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="J28" s="1">
+        <v>11</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="V28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X28" s="1">
+        <v>11</v>
+      </c>
+      <c r="Y28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z28" s="5">
+        <v>37867</v>
+      </c>
+      <c r="AA28" s="1"/>
+      <c r="AB28" s="1"/>
+      <c r="AC28" s="1"/>
+      <c r="AD28" s="1"/>
+      <c r="AE28" s="1"/>
+    </row>
+    <row r="29" spans="1:31">
+      <c r="A29" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1</v>
+      </c>
+      <c r="C29" s="1">
+        <v>1</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F29" s="1"/>
+      <c r="G29" s="4">
+        <v>35738</v>
+      </c>
+      <c r="H29" s="1">
+        <v>119990004</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="J29" s="1">
+        <v>11</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="R29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="V29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X29" s="1">
+        <v>11</v>
+      </c>
+      <c r="Y29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z29" s="5">
+        <v>37868</v>
+      </c>
+      <c r="AA29" s="1"/>
+      <c r="AB29" s="1"/>
+      <c r="AC29" s="1"/>
+      <c r="AD29" s="1"/>
+      <c r="AE29" s="1"/>
+    </row>
+    <row r="30" spans="1:31">
+      <c r="A30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="1">
+        <v>1</v>
+      </c>
+      <c r="C30" s="1">
+        <v>1</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G30" s="4">
+        <v>35739</v>
+      </c>
+      <c r="H30" s="1">
+        <v>119990005</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="J30" s="1">
+        <v>11</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="T30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="V30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X30" s="1">
+        <v>11</v>
+      </c>
+      <c r="Y30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z30" s="5">
+        <v>37869</v>
+      </c>
+      <c r="AA30" s="1"/>
+      <c r="AB30" s="1"/>
+      <c r="AC30" s="1"/>
+      <c r="AD30" s="1"/>
+      <c r="AE30" s="1"/>
+    </row>
+    <row r="31" spans="1:31">
+      <c r="A31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1</v>
+      </c>
+      <c r="C31" s="1">
+        <v>1</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F31" s="1"/>
+      <c r="G31" s="4">
+        <v>35740</v>
+      </c>
+      <c r="H31" s="1">
+        <v>119990006</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="J31" s="1">
+        <v>11</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="V31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X31" s="1">
+        <v>11</v>
+      </c>
+      <c r="Y31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z31" s="5">
+        <v>37870</v>
+      </c>
+      <c r="AA31" s="1"/>
+      <c r="AB31" s="1"/>
+      <c r="AC31" s="1"/>
+      <c r="AD31" s="1"/>
+      <c r="AE31" s="1"/>
+    </row>
+    <row r="32" spans="1:31">
+      <c r="A32" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="1">
+        <v>1</v>
+      </c>
+      <c r="C32" s="1">
+        <v>1</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F32" s="1"/>
+      <c r="G32" s="4">
+        <v>35741</v>
+      </c>
+      <c r="H32" s="1">
+        <v>119990007</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="J32" s="1">
+        <v>11</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="V32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X32" s="1">
+        <v>11</v>
+      </c>
+      <c r="Y32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z32" s="5">
+        <v>37871</v>
+      </c>
+      <c r="AA32" s="1"/>
+      <c r="AB32" s="1"/>
+      <c r="AC32" s="1"/>
+      <c r="AD32" s="1"/>
+      <c r="AE32" s="1"/>
+    </row>
+    <row r="33" spans="1:31">
+      <c r="A33" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="1">
+        <v>1</v>
+      </c>
+      <c r="C33" s="1">
+        <v>1</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F33" s="1"/>
+      <c r="G33" s="4">
+        <v>35742</v>
+      </c>
+      <c r="H33" s="1">
+        <v>119990008</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="J33" s="1">
+        <v>11</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="R33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="V33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X33" s="1">
+        <v>11</v>
+      </c>
+      <c r="Y33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z33" s="5">
+        <v>37872</v>
+      </c>
+      <c r="AA33" s="1"/>
+      <c r="AB33" s="1"/>
+      <c r="AC33" s="1"/>
+      <c r="AD33" s="1"/>
+      <c r="AE33" s="1"/>
+    </row>
+    <row r="34" spans="1:31">
+      <c r="A34" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="1">
+        <v>1</v>
+      </c>
+      <c r="C34" s="1">
+        <v>1</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G34" s="4">
+        <v>35743</v>
+      </c>
+      <c r="H34" s="1">
+        <v>119990009</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="J34" s="1">
+        <v>11</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="T34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="V34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X34" s="1">
+        <v>11</v>
+      </c>
+      <c r="Y34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z34" s="5">
+        <v>37873</v>
+      </c>
+      <c r="AA34" s="1"/>
+      <c r="AB34" s="1"/>
+      <c r="AC34" s="1"/>
+      <c r="AD34" s="1"/>
+      <c r="AE34" s="1"/>
+    </row>
+    <row r="35" spans="1:31">
+      <c r="A35" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="1">
+        <v>1</v>
+      </c>
+      <c r="C35" s="1">
+        <v>1</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F35" s="1"/>
+      <c r="G35" s="4">
+        <v>35744</v>
+      </c>
+      <c r="H35" s="1">
+        <v>119990010</v>
+      </c>
+      <c r="I35" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="J35" s="1">
+        <v>11</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="V35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X35" s="1">
+        <v>11</v>
+      </c>
+      <c r="Y35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z35" s="5">
+        <v>37874</v>
+      </c>
+      <c r="AA35" s="1"/>
+      <c r="AB35" s="1"/>
+      <c r="AC35" s="1"/>
+      <c r="AD35" s="1"/>
+      <c r="AE35" s="1"/>
+    </row>
+    <row r="36" spans="1:31">
+      <c r="A36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="1">
+        <v>1</v>
+      </c>
+      <c r="C36" s="1">
+        <v>1</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F36" s="1"/>
+      <c r="G36" s="4">
+        <v>35745</v>
+      </c>
+      <c r="H36" s="1">
+        <v>119990011</v>
+      </c>
+      <c r="I36" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="J36" s="1">
+        <v>11</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U36" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="V36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X36" s="1">
+        <v>11</v>
+      </c>
+      <c r="Y36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z36" s="5">
+        <v>37875</v>
+      </c>
+      <c r="AA36" s="1"/>
+      <c r="AB36" s="1"/>
+      <c r="AC36" s="1"/>
+      <c r="AD36" s="1"/>
+      <c r="AE36" s="1"/>
+    </row>
+    <row r="37" spans="1:31">
+      <c r="A37" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" s="1">
+        <v>1</v>
+      </c>
+      <c r="C37" s="1">
+        <v>1</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F37" s="1"/>
+      <c r="G37" s="4">
+        <v>35746</v>
+      </c>
+      <c r="H37" s="1">
+        <v>119990012</v>
+      </c>
+      <c r="I37" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="J37" s="1">
+        <v>11</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q37" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="R37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="V37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X37" s="1">
+        <v>11</v>
+      </c>
+      <c r="Y37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z37" s="5">
+        <v>37876</v>
+      </c>
+      <c r="AA37" s="1"/>
+      <c r="AB37" s="1"/>
+      <c r="AC37" s="1"/>
+      <c r="AD37" s="1"/>
+      <c r="AE37" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Updated analysis for ExamineeAttributes so that maximum width, is required, and is optional information about the fields is calculated.
</commit_message>
<xml_diff>
--- a/irp-webapp/src/main/resources/irp-package/IRPStudents.xlsx
+++ b/irp-webapp/src/main/resources/irp-package/IRPStudents.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="23460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="STUDENT" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="159">
   <si>
     <t>SSID</t>
   </si>
@@ -490,6 +490,12 @@
   </si>
   <si>
     <t>MiddleAG</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>07</t>
   </si>
 </sst>
 </file>
@@ -606,15 +612,34 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="59">
@@ -1007,113 +1032,118 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="AA14" sqref="AA14"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="4"/>
+    <col min="2" max="2" width="24.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="10.83203125" style="4"/>
+    <col min="10" max="10" width="10.83203125" style="2"/>
+    <col min="11" max="22" width="10.83203125" style="4"/>
+    <col min="23" max="23" width="13.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="27.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.83203125" style="4"/>
+    <col min="26" max="26" width="24.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="29.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="10.83203125" style="4"/>
+    <col min="30" max="30" width="18.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="18.33203125" style="4" customWidth="1"/>
+    <col min="32" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:31" s="9" customFormat="1">
+      <c r="A1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1" s="3" t="s">
+      <c r="K1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="U1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="V1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="W1" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="X1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Y1" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="Z1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AA1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AB1" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AC1" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AD1" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AE1" s="8" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1136,17 +1166,17 @@
       <c r="F2" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="5">
         <v>39508</v>
       </c>
       <c r="H2" s="1">
         <v>39990001</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="J2" s="1">
-        <v>3</v>
+      <c r="J2" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>5</v>
@@ -1193,7 +1223,7 @@
       <c r="Y2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Z2" s="5">
+      <c r="Z2" s="6">
         <v>40393</v>
       </c>
       <c r="AA2" s="1"/>
@@ -1219,17 +1249,17 @@
         <v>41</v>
       </c>
       <c r="F3" s="1"/>
-      <c r="G3" s="4">
+      <c r="G3" s="5">
         <v>39509</v>
       </c>
       <c r="H3" s="1">
         <v>39990002</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J3" s="1">
-        <v>3</v>
+      <c r="J3" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>5</v>
@@ -1276,7 +1306,7 @@
       <c r="Y3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Z3" s="5">
+      <c r="Z3" s="6">
         <v>40394</v>
       </c>
       <c r="AA3" s="1"/>
@@ -1302,17 +1332,17 @@
         <v>42</v>
       </c>
       <c r="F4" s="1"/>
-      <c r="G4" s="4">
+      <c r="G4" s="5">
         <v>39510</v>
       </c>
       <c r="H4" s="1">
         <v>39990003</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="J4" s="1">
-        <v>3</v>
+      <c r="J4" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>9</v>
@@ -1359,7 +1389,7 @@
       <c r="Y4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Z4" s="5">
+      <c r="Z4" s="6">
         <v>40395</v>
       </c>
       <c r="AA4" s="1"/>
@@ -1385,17 +1415,17 @@
         <v>43</v>
       </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="4">
+      <c r="G5" s="5">
         <v>39511</v>
       </c>
       <c r="H5" s="1">
         <v>39990004</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="J5" s="1">
-        <v>3</v>
+      <c r="J5" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>9</v>
@@ -1442,16 +1472,16 @@
       <c r="Y5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Z5" s="5">
+      <c r="Z5" s="6">
         <v>40396</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AA5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AB5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AC5" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1474,17 +1504,17 @@
       <c r="F6" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="5">
         <v>39512</v>
       </c>
       <c r="H6" s="1">
         <v>39990005</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="J6" s="1">
-        <v>3</v>
+      <c r="J6" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>5</v>
@@ -1531,7 +1561,7 @@
       <c r="Y6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Z6" s="5">
+      <c r="Z6" s="6">
         <v>40397</v>
       </c>
       <c r="AA6" s="1"/>
@@ -1557,17 +1587,17 @@
         <v>57</v>
       </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="4">
+      <c r="G7" s="5">
         <v>39513</v>
       </c>
       <c r="H7" s="1">
         <v>39990006</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="J7" s="1">
-        <v>3</v>
+      <c r="J7" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>5</v>
@@ -1614,7 +1644,7 @@
       <c r="Y7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Z7" s="5">
+      <c r="Z7" s="6">
         <v>40398</v>
       </c>
       <c r="AA7" s="1"/>
@@ -1640,17 +1670,17 @@
         <v>58</v>
       </c>
       <c r="F8" s="1"/>
-      <c r="G8" s="4">
+      <c r="G8" s="5">
         <v>39514</v>
       </c>
       <c r="H8" s="1">
         <v>39990007</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="I8" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="J8" s="1">
-        <v>3</v>
+      <c r="J8" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>9</v>
@@ -1697,7 +1727,7 @@
       <c r="Y8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Z8" s="5">
+      <c r="Z8" s="6">
         <v>40399</v>
       </c>
       <c r="AA8" s="1"/>
@@ -1723,17 +1753,17 @@
         <v>59</v>
       </c>
       <c r="F9" s="1"/>
-      <c r="G9" s="4">
+      <c r="G9" s="5">
         <v>39515</v>
       </c>
       <c r="H9" s="1">
         <v>39990008</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="I9" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="J9" s="1">
-        <v>3</v>
+      <c r="J9" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>9</v>
@@ -1780,16 +1810,16 @@
       <c r="Y9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Z9" s="5">
+      <c r="Z9" s="6">
         <v>40400</v>
       </c>
-      <c r="AA9" t="s">
+      <c r="AA9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="AB9" t="s">
+      <c r="AB9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="AC9" t="s">
+      <c r="AC9" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1812,17 +1842,17 @@
       <c r="F10" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="5">
         <v>39516</v>
       </c>
       <c r="H10" s="1">
         <v>39990009</v>
       </c>
-      <c r="I10" s="6" t="s">
+      <c r="I10" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="J10" s="1">
-        <v>3</v>
+      <c r="J10" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>5</v>
@@ -1869,7 +1899,7 @@
       <c r="Y10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Z10" s="5">
+      <c r="Z10" s="6">
         <v>40401</v>
       </c>
       <c r="AA10" s="1"/>
@@ -1895,17 +1925,17 @@
         <v>61</v>
       </c>
       <c r="F11" s="1"/>
-      <c r="G11" s="4">
+      <c r="G11" s="5">
         <v>39517</v>
       </c>
       <c r="H11" s="1">
         <v>39990010</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="I11" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="J11" s="1">
-        <v>3</v>
+      <c r="J11" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>5</v>
@@ -1952,7 +1982,7 @@
       <c r="Y11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Z11" s="5">
+      <c r="Z11" s="6">
         <v>40402</v>
       </c>
       <c r="AA11" s="1"/>
@@ -1978,17 +2008,17 @@
         <v>62</v>
       </c>
       <c r="F12" s="1"/>
-      <c r="G12" s="4">
+      <c r="G12" s="5">
         <v>39518</v>
       </c>
       <c r="H12" s="1">
         <v>39990011</v>
       </c>
-      <c r="I12" s="6" t="s">
+      <c r="I12" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="J12" s="1">
-        <v>3</v>
+      <c r="J12" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>9</v>
@@ -2035,7 +2065,7 @@
       <c r="Y12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Z12" s="5">
+      <c r="Z12" s="6">
         <v>40403</v>
       </c>
       <c r="AA12" s="1"/>
@@ -2061,17 +2091,17 @@
         <v>63</v>
       </c>
       <c r="F13" s="1"/>
-      <c r="G13" s="4">
+      <c r="G13" s="5">
         <v>39519</v>
       </c>
       <c r="H13" s="1">
         <v>39990012</v>
       </c>
-      <c r="I13" s="6" t="s">
+      <c r="I13" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="J13" s="1">
-        <v>3</v>
+      <c r="J13" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>9</v>
@@ -2118,16 +2148,16 @@
       <c r="Y13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Z13" s="5">
+      <c r="Z13" s="6">
         <v>40404</v>
       </c>
-      <c r="AA13" t="s">
+      <c r="AA13" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="AB13" t="s">
+      <c r="AB13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="AC13" t="s">
+      <c r="AC13" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2148,17 +2178,17 @@
         <v>76</v>
       </c>
       <c r="F14" s="1"/>
-      <c r="G14" s="4">
+      <c r="G14" s="5">
         <v>38169</v>
       </c>
       <c r="H14" s="1">
         <v>79990001</v>
       </c>
-      <c r="I14" s="6" t="s">
+      <c r="I14" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="J14" s="1">
-        <v>7</v>
+      <c r="J14" s="3" t="s">
+        <v>158</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>5</v>
@@ -2205,10 +2235,10 @@
       <c r="Y14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Z14" s="5">
+      <c r="Z14" s="6">
         <v>38961</v>
       </c>
-      <c r="AA14" s="2"/>
+      <c r="AA14" s="7"/>
       <c r="AB14" s="1"/>
       <c r="AC14" s="1"/>
       <c r="AD14" s="1"/>
@@ -2233,17 +2263,17 @@
       <c r="F15" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="5">
         <v>38170</v>
       </c>
       <c r="H15" s="1">
         <v>79990002</v>
       </c>
-      <c r="I15" s="6" t="s">
+      <c r="I15" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="J15" s="1">
-        <v>7</v>
+      <c r="J15" s="3" t="s">
+        <v>158</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>9</v>
@@ -2290,7 +2320,7 @@
       <c r="Y15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Z15" s="5">
+      <c r="Z15" s="6">
         <v>38962</v>
       </c>
       <c r="AA15" s="1"/>
@@ -2316,17 +2346,17 @@
         <v>78</v>
       </c>
       <c r="F16" s="1"/>
-      <c r="G16" s="4">
+      <c r="G16" s="5">
         <v>38171</v>
       </c>
       <c r="H16" s="1">
         <v>79990003</v>
       </c>
-      <c r="I16" s="6" t="s">
+      <c r="I16" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="J16" s="1">
-        <v>7</v>
+      <c r="J16" s="3" t="s">
+        <v>158</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>5</v>
@@ -2373,7 +2403,7 @@
       <c r="Y16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Z16" s="5">
+      <c r="Z16" s="6">
         <v>38963</v>
       </c>
       <c r="AA16" s="1"/>
@@ -2399,17 +2429,17 @@
         <v>79</v>
       </c>
       <c r="F17" s="1"/>
-      <c r="G17" s="4">
+      <c r="G17" s="5">
         <v>38172</v>
       </c>
       <c r="H17" s="1">
         <v>79990004</v>
       </c>
-      <c r="I17" s="6" t="s">
+      <c r="I17" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="J17" s="1">
-        <v>7</v>
+      <c r="J17" s="3" t="s">
+        <v>158</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>5</v>
@@ -2456,7 +2486,7 @@
       <c r="Y17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Z17" s="5">
+      <c r="Z17" s="6">
         <v>38964</v>
       </c>
       <c r="AA17" s="1"/>
@@ -2482,17 +2512,17 @@
         <v>80</v>
       </c>
       <c r="F18" s="1"/>
-      <c r="G18" s="4">
+      <c r="G18" s="5">
         <v>38173</v>
       </c>
       <c r="H18" s="1">
         <v>79990005</v>
       </c>
-      <c r="I18" s="6" t="s">
+      <c r="I18" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="J18" s="1">
-        <v>7</v>
+      <c r="J18" s="3" t="s">
+        <v>158</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>5</v>
@@ -2539,10 +2569,10 @@
       <c r="Y18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Z18" s="5">
+      <c r="Z18" s="6">
         <v>38965</v>
       </c>
-      <c r="AA18" s="2"/>
+      <c r="AA18" s="7"/>
       <c r="AB18" s="1"/>
       <c r="AC18" s="1"/>
       <c r="AD18" s="1"/>
@@ -2567,17 +2597,17 @@
       <c r="F19" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="5">
         <v>38174</v>
       </c>
       <c r="H19" s="1">
         <v>79990006</v>
       </c>
-      <c r="I19" s="6" t="s">
+      <c r="I19" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="J19" s="1">
-        <v>7</v>
+      <c r="J19" s="3" t="s">
+        <v>158</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>9</v>
@@ -2624,7 +2654,7 @@
       <c r="Y19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Z19" s="5">
+      <c r="Z19" s="6">
         <v>38966</v>
       </c>
       <c r="AA19" s="1"/>
@@ -2650,17 +2680,17 @@
         <v>82</v>
       </c>
       <c r="F20" s="1"/>
-      <c r="G20" s="4">
+      <c r="G20" s="5">
         <v>38175</v>
       </c>
       <c r="H20" s="1">
         <v>79990007</v>
       </c>
-      <c r="I20" s="6" t="s">
+      <c r="I20" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="J20" s="1">
-        <v>7</v>
+      <c r="J20" s="3" t="s">
+        <v>158</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>5</v>
@@ -2707,7 +2737,7 @@
       <c r="Y20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Z20" s="5">
+      <c r="Z20" s="6">
         <v>38967</v>
       </c>
       <c r="AA20" s="1"/>
@@ -2733,17 +2763,17 @@
         <v>83</v>
       </c>
       <c r="F21" s="1"/>
-      <c r="G21" s="4">
+      <c r="G21" s="5">
         <v>38176</v>
       </c>
       <c r="H21" s="1">
         <v>79990008</v>
       </c>
-      <c r="I21" s="6" t="s">
+      <c r="I21" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="J21" s="1">
-        <v>7</v>
+      <c r="J21" s="3" t="s">
+        <v>158</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>5</v>
@@ -2790,7 +2820,7 @@
       <c r="Y21" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Z21" s="5">
+      <c r="Z21" s="6">
         <v>38968</v>
       </c>
       <c r="AA21" s="1"/>
@@ -2816,17 +2846,17 @@
         <v>84</v>
       </c>
       <c r="F22" s="1"/>
-      <c r="G22" s="4">
+      <c r="G22" s="5">
         <v>38177</v>
       </c>
       <c r="H22" s="1">
         <v>79990009</v>
       </c>
-      <c r="I22" s="6" t="s">
+      <c r="I22" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="J22" s="1">
-        <v>7</v>
+      <c r="J22" s="3" t="s">
+        <v>158</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>5</v>
@@ -2873,10 +2903,10 @@
       <c r="Y22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Z22" s="5">
+      <c r="Z22" s="6">
         <v>38969</v>
       </c>
-      <c r="AA22" s="2"/>
+      <c r="AA22" s="7"/>
       <c r="AB22" s="1"/>
       <c r="AC22" s="1"/>
       <c r="AD22" s="1"/>
@@ -2901,17 +2931,17 @@
       <c r="F23" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G23" s="5">
         <v>38178</v>
       </c>
       <c r="H23" s="1">
         <v>79990010</v>
       </c>
-      <c r="I23" s="6" t="s">
+      <c r="I23" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="J23" s="1">
-        <v>7</v>
+      <c r="J23" s="3" t="s">
+        <v>158</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>9</v>
@@ -2958,7 +2988,7 @@
       <c r="Y23" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Z23" s="5">
+      <c r="Z23" s="6">
         <v>38970</v>
       </c>
       <c r="AA23" s="1"/>
@@ -2984,17 +3014,17 @@
         <v>86</v>
       </c>
       <c r="F24" s="1"/>
-      <c r="G24" s="4">
+      <c r="G24" s="5">
         <v>38179</v>
       </c>
       <c r="H24" s="1">
         <v>79990011</v>
       </c>
-      <c r="I24" s="6" t="s">
+      <c r="I24" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="J24" s="1">
-        <v>7</v>
+      <c r="J24" s="3" t="s">
+        <v>158</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>5</v>
@@ -3041,7 +3071,7 @@
       <c r="Y24" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Z24" s="5">
+      <c r="Z24" s="6">
         <v>38971</v>
       </c>
       <c r="AA24" s="1"/>
@@ -3067,17 +3097,17 @@
         <v>87</v>
       </c>
       <c r="F25" s="1"/>
-      <c r="G25" s="4">
+      <c r="G25" s="5">
         <v>38180</v>
       </c>
       <c r="H25" s="1">
         <v>79990012</v>
       </c>
-      <c r="I25" s="6" t="s">
+      <c r="I25" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="J25" s="1">
-        <v>7</v>
+      <c r="J25" s="3" t="s">
+        <v>158</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>5</v>
@@ -3124,7 +3154,7 @@
       <c r="Y25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Z25" s="5">
+      <c r="Z25" s="6">
         <v>38972</v>
       </c>
       <c r="AA25" s="1"/>
@@ -3152,16 +3182,16 @@
       <c r="F26" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G26" s="4">
+      <c r="G26" s="5">
         <v>35735</v>
       </c>
       <c r="H26" s="1">
         <v>119990001</v>
       </c>
-      <c r="I26" s="6" t="s">
+      <c r="I26" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="J26" s="1">
+      <c r="J26" s="3">
         <v>11</v>
       </c>
       <c r="K26" s="1" t="s">
@@ -3209,7 +3239,7 @@
       <c r="Y26" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Z26" s="5">
+      <c r="Z26" s="6">
         <v>37865</v>
       </c>
       <c r="AA26" s="1"/>
@@ -3235,16 +3265,16 @@
         <v>101</v>
       </c>
       <c r="F27" s="1"/>
-      <c r="G27" s="4">
+      <c r="G27" s="5">
         <v>35736</v>
       </c>
       <c r="H27" s="1">
         <v>119990002</v>
       </c>
-      <c r="I27" s="6" t="s">
+      <c r="I27" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="J27" s="1">
+      <c r="J27" s="3">
         <v>11</v>
       </c>
       <c r="K27" s="1" t="s">
@@ -3292,7 +3322,7 @@
       <c r="Y27" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Z27" s="5">
+      <c r="Z27" s="6">
         <v>37866</v>
       </c>
       <c r="AA27" s="1"/>
@@ -3318,16 +3348,16 @@
         <v>102</v>
       </c>
       <c r="F28" s="1"/>
-      <c r="G28" s="4">
+      <c r="G28" s="5">
         <v>35737</v>
       </c>
       <c r="H28" s="1">
         <v>119990003</v>
       </c>
-      <c r="I28" s="6" t="s">
+      <c r="I28" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="J28" s="1">
+      <c r="J28" s="3">
         <v>11</v>
       </c>
       <c r="K28" s="1" t="s">
@@ -3375,7 +3405,7 @@
       <c r="Y28" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Z28" s="5">
+      <c r="Z28" s="6">
         <v>37867</v>
       </c>
       <c r="AA28" s="1"/>
@@ -3401,16 +3431,16 @@
         <v>103</v>
       </c>
       <c r="F29" s="1"/>
-      <c r="G29" s="4">
+      <c r="G29" s="5">
         <v>35738</v>
       </c>
       <c r="H29" s="1">
         <v>119990004</v>
       </c>
-      <c r="I29" s="6" t="s">
+      <c r="I29" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="J29" s="1">
+      <c r="J29" s="3">
         <v>11</v>
       </c>
       <c r="K29" s="1" t="s">
@@ -3458,7 +3488,7 @@
       <c r="Y29" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Z29" s="5">
+      <c r="Z29" s="6">
         <v>37868</v>
       </c>
       <c r="AA29" s="1"/>
@@ -3486,16 +3516,16 @@
       <c r="F30" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="G30" s="4">
+      <c r="G30" s="5">
         <v>35739</v>
       </c>
       <c r="H30" s="1">
         <v>119990005</v>
       </c>
-      <c r="I30" s="6" t="s">
+      <c r="I30" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="J30" s="1">
+      <c r="J30" s="3">
         <v>11</v>
       </c>
       <c r="K30" s="1" t="s">
@@ -3543,7 +3573,7 @@
       <c r="Y30" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Z30" s="5">
+      <c r="Z30" s="6">
         <v>37869</v>
       </c>
       <c r="AA30" s="1"/>
@@ -3569,16 +3599,16 @@
         <v>105</v>
       </c>
       <c r="F31" s="1"/>
-      <c r="G31" s="4">
+      <c r="G31" s="5">
         <v>35740</v>
       </c>
       <c r="H31" s="1">
         <v>119990006</v>
       </c>
-      <c r="I31" s="6" t="s">
+      <c r="I31" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="J31" s="1">
+      <c r="J31" s="3">
         <v>11</v>
       </c>
       <c r="K31" s="1" t="s">
@@ -3626,7 +3656,7 @@
       <c r="Y31" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Z31" s="5">
+      <c r="Z31" s="6">
         <v>37870</v>
       </c>
       <c r="AA31" s="1"/>
@@ -3652,16 +3682,16 @@
         <v>106</v>
       </c>
       <c r="F32" s="1"/>
-      <c r="G32" s="4">
+      <c r="G32" s="5">
         <v>35741</v>
       </c>
       <c r="H32" s="1">
         <v>119990007</v>
       </c>
-      <c r="I32" s="6" t="s">
+      <c r="I32" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="J32" s="1">
+      <c r="J32" s="3">
         <v>11</v>
       </c>
       <c r="K32" s="1" t="s">
@@ -3709,7 +3739,7 @@
       <c r="Y32" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Z32" s="5">
+      <c r="Z32" s="6">
         <v>37871</v>
       </c>
       <c r="AA32" s="1"/>
@@ -3735,16 +3765,16 @@
         <v>107</v>
       </c>
       <c r="F33" s="1"/>
-      <c r="G33" s="4">
+      <c r="G33" s="5">
         <v>35742</v>
       </c>
       <c r="H33" s="1">
         <v>119990008</v>
       </c>
-      <c r="I33" s="6" t="s">
+      <c r="I33" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="J33" s="1">
+      <c r="J33" s="3">
         <v>11</v>
       </c>
       <c r="K33" s="1" t="s">
@@ -3792,7 +3822,7 @@
       <c r="Y33" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Z33" s="5">
+      <c r="Z33" s="6">
         <v>37872</v>
       </c>
       <c r="AA33" s="1"/>
@@ -3820,16 +3850,16 @@
       <c r="F34" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="G34" s="4">
+      <c r="G34" s="5">
         <v>35743</v>
       </c>
       <c r="H34" s="1">
         <v>119990009</v>
       </c>
-      <c r="I34" s="6" t="s">
+      <c r="I34" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="J34" s="1">
+      <c r="J34" s="3">
         <v>11</v>
       </c>
       <c r="K34" s="1" t="s">
@@ -3877,7 +3907,7 @@
       <c r="Y34" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Z34" s="5">
+      <c r="Z34" s="6">
         <v>37873</v>
       </c>
       <c r="AA34" s="1"/>
@@ -3903,16 +3933,16 @@
         <v>109</v>
       </c>
       <c r="F35" s="1"/>
-      <c r="G35" s="4">
+      <c r="G35" s="5">
         <v>35744</v>
       </c>
       <c r="H35" s="1">
         <v>119990010</v>
       </c>
-      <c r="I35" s="6" t="s">
+      <c r="I35" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="J35" s="1">
+      <c r="J35" s="3">
         <v>11</v>
       </c>
       <c r="K35" s="1" t="s">
@@ -3960,7 +3990,7 @@
       <c r="Y35" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Z35" s="5">
+      <c r="Z35" s="6">
         <v>37874</v>
       </c>
       <c r="AA35" s="1"/>
@@ -3986,16 +4016,16 @@
         <v>110</v>
       </c>
       <c r="F36" s="1"/>
-      <c r="G36" s="4">
+      <c r="G36" s="5">
         <v>35745</v>
       </c>
       <c r="H36" s="1">
         <v>119990011</v>
       </c>
-      <c r="I36" s="6" t="s">
+      <c r="I36" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="J36" s="1">
+      <c r="J36" s="3">
         <v>11</v>
       </c>
       <c r="K36" s="1" t="s">
@@ -4043,7 +4073,7 @@
       <c r="Y36" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Z36" s="5">
+      <c r="Z36" s="6">
         <v>37875</v>
       </c>
       <c r="AA36" s="1"/>
@@ -4069,16 +4099,16 @@
         <v>111</v>
       </c>
       <c r="F37" s="1"/>
-      <c r="G37" s="4">
+      <c r="G37" s="5">
         <v>35746</v>
       </c>
       <c r="H37" s="1">
         <v>119990012</v>
       </c>
-      <c r="I37" s="6" t="s">
+      <c r="I37" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="J37" s="1">
+      <c r="J37" s="3">
         <v>11</v>
       </c>
       <c r="K37" s="1" t="s">
@@ -4126,7 +4156,7 @@
       <c r="Y37" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Z37" s="5">
+      <c r="Z37" s="6">
         <v>37876</v>
       </c>
       <c r="AA37" s="1"/>
@@ -4138,6 +4168,9 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <ignoredErrors>
+    <ignoredError sqref="J2 J3:J25" numberStoredAsText="1"/>
+  </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Made further updates to ExamineeAttributes and changed the report format of the UI to contain only four columns with the error explanation below the row.
</commit_message>
<xml_diff>
--- a/irp-webapp/src/main/resources/irp-package/IRPStudents.xlsx
+++ b/irp-webapp/src/main/resources/irp-package/IRPStudents.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="20" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="STUDENT" sheetId="1" r:id="rId1"/>
@@ -39,12 +39,6 @@
     <t>Male</t>
   </si>
   <si>
-    <t>YES</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
     <t>eng</t>
   </si>
   <si>
@@ -87,18 +81,9 @@
     <t>GradeLevelWhenAssessed</t>
   </si>
   <si>
-    <t>HispanicOrLatinoEthnicity</t>
-  </si>
-  <si>
-    <t>AmericanIndianOrAlaskaNative</t>
-  </si>
-  <si>
     <t>BlackOrAfricanAmerican</t>
   </si>
   <si>
-    <t>NativeHawaiianOrOtherPacificIslander</t>
-  </si>
-  <si>
     <t>DemographicRaceTwoOrMoreRaces</t>
   </si>
   <si>
@@ -111,9 +96,6 @@
     <t>Section504Status</t>
   </si>
   <si>
-    <t>EconomicDisadvantageStatus</t>
-  </si>
-  <si>
     <t>LanguageCode</t>
   </si>
   <si>
@@ -496,6 +478,24 @@
   </si>
   <si>
     <t>07</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>HispanicOrLatiNoEthnicity</t>
+  </si>
+  <si>
+    <t>AmericanIndiaNorAlaskaNative</t>
+  </si>
+  <si>
+    <t>NativeHawaiiaNorOtherPacificIslander</t>
+  </si>
+  <si>
+    <t>EcoNomicDisadvantageStatus</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -1032,7 +1032,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="AD1" sqref="AD1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -1054,97 +1056,97 @@
   <sheetData>
     <row r="1" spans="1:31" s="9" customFormat="1">
       <c r="A1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>17</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>19</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>22</v>
+        <v>154</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>23</v>
+        <v>155</v>
       </c>
       <c r="N1" s="8" t="s">
         <v>2</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="P1" s="8" t="s">
         <v>3</v>
       </c>
       <c r="Q1" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="R1" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="T1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="U1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="V1" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="W1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="X1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="Y1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="Z1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="AA1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="AB1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="AC1" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="AD1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="AE1" s="8" t="s">
         <v>33</v>
-      </c>
-      <c r="Z1" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA1" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB1" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC1" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD1" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="AE1" s="8" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:31">
@@ -1158,13 +1160,13 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="G2" s="5">
         <v>39508</v>
@@ -1173,55 +1175,55 @@
         <v>39990001</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="W2" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="X2" s="1">
         <v>3</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="Z2" s="6">
         <v>40393</v>
@@ -1243,10 +1245,10 @@
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="5">
@@ -1256,55 +1258,55 @@
         <v>39990002</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="N3" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="W3" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="X3" s="1">
         <v>3</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="Z3" s="6">
         <v>40394</v>
@@ -1326,10 +1328,10 @@
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="5">
@@ -1339,55 +1341,55 @@
         <v>39990003</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="O4" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="W4" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="X4" s="1">
         <v>3</v>
       </c>
       <c r="Y4" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="Z4" s="6">
         <v>40395</v>
@@ -1409,10 +1411,10 @@
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="5">
@@ -1422,67 +1424,67 @@
         <v>39990004</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="P5" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="W5" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="V5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="W5" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="X5" s="1">
         <v>3</v>
       </c>
       <c r="Y5" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="Z5" s="6">
         <v>40396</v>
       </c>
       <c r="AA5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC5" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="AB5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC5" s="4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:31">
@@ -1496,13 +1498,13 @@
         <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="G6" s="5">
         <v>39512</v>
@@ -1511,55 +1513,55 @@
         <v>39990005</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="L6" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="W6" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="T6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="V6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="W6" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="X6" s="1">
         <v>3</v>
       </c>
       <c r="Y6" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="Z6" s="6">
         <v>40397</v>
@@ -1581,10 +1583,10 @@
         <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="5">
@@ -1594,55 +1596,55 @@
         <v>39990006</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="N7" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="W7" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="R7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="S7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="T7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="U7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="V7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="W7" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="X7" s="1">
         <v>3</v>
       </c>
       <c r="Y7" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="Z7" s="6">
         <v>40398</v>
@@ -1664,10 +1666,10 @@
         <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="5">
@@ -1677,55 +1679,55 @@
         <v>39990007</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="O8" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="W8" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="S8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="T8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="U8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="V8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="W8" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="X8" s="1">
         <v>3</v>
       </c>
       <c r="Y8" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="Z8" s="6">
         <v>40399</v>
@@ -1747,10 +1749,10 @@
         <v>1</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="5">
@@ -1760,67 +1762,67 @@
         <v>39990008</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="P9" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="W9" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="Q9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="R9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="S9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="T9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="U9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="V9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="W9" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="X9" s="1">
         <v>3</v>
       </c>
       <c r="Y9" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="Z9" s="6">
         <v>40400</v>
       </c>
       <c r="AA9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC9" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="AB9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC9" s="4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:31">
@@ -1834,13 +1836,13 @@
         <v>1</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="G10" s="5">
         <v>39516</v>
@@ -1849,55 +1851,55 @@
         <v>39990009</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>5</v>
       </c>
       <c r="L10" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="W10" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="R10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="S10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="T10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="U10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="V10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="W10" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="X10" s="1">
         <v>3</v>
       </c>
       <c r="Y10" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="Z10" s="6">
         <v>40401</v>
@@ -1919,10 +1921,10 @@
         <v>1</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="5">
@@ -1932,55 +1934,55 @@
         <v>39990010</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="N11" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="W11" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="R11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="S11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="T11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="U11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="V11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="W11" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="X11" s="1">
         <v>3</v>
       </c>
       <c r="Y11" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="Z11" s="6">
         <v>40402</v>
@@ -2002,10 +2004,10 @@
         <v>1</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="5">
@@ -2015,55 +2017,55 @@
         <v>39990011</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="O12" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="U12" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="V12" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="W12" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="R12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="S12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="T12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="U12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="V12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="W12" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="X12" s="1">
         <v>3</v>
       </c>
       <c r="Y12" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="Z12" s="6">
         <v>40403</v>
@@ -2085,10 +2087,10 @@
         <v>1</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="5">
@@ -2098,67 +2100,67 @@
         <v>39990012</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="P13" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="T13" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="U13" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="V13" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="W13" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="Q13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="R13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="S13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="T13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="U13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="V13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="W13" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="X13" s="1">
         <v>3</v>
       </c>
       <c r="Y13" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="Z13" s="6">
         <v>40404</v>
       </c>
       <c r="AA13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC13" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="AB13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC13" s="4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:31">
@@ -2172,10 +2174,10 @@
         <v>1</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="5">
@@ -2185,55 +2187,55 @@
         <v>79990001</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>5</v>
       </c>
       <c r="L14" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="T14" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="U14" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="V14" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="W14" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="O14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="R14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="T14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="U14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="V14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="W14" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="X14" s="1">
         <v>7</v>
       </c>
       <c r="Y14" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="Z14" s="6">
         <v>38961</v>
@@ -2255,13 +2257,13 @@
         <v>1</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="G15" s="5">
         <v>38170</v>
@@ -2270,55 +2272,55 @@
         <v>79990002</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="M15" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="R15" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="S15" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="T15" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="U15" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="V15" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="W15" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="R15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="S15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="T15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="U15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="V15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="W15" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="X15" s="1">
         <v>7</v>
       </c>
       <c r="Y15" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="Z15" s="6">
         <v>38962</v>
@@ -2340,10 +2342,10 @@
         <v>1</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="5">
@@ -2353,55 +2355,55 @@
         <v>79990003</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>5</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="N16" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="T16" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="U16" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="V16" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="W16" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="O16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="R16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="S16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="T16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="U16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="V16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="W16" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="X16" s="1">
         <v>7</v>
       </c>
       <c r="Y16" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="Z16" s="6">
         <v>38963</v>
@@ -2423,10 +2425,10 @@
         <v>1</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="5">
@@ -2436,55 +2438,55 @@
         <v>79990004</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>5</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="N17" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="S17" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="T17" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="U17" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="V17" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="W17" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="O17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="R17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="S17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="T17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="U17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="V17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="W17" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="X17" s="1">
         <v>7</v>
       </c>
       <c r="Y17" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="Z17" s="6">
         <v>38964</v>
@@ -2506,10 +2508,10 @@
         <v>1</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="5">
@@ -2519,55 +2521,55 @@
         <v>79990005</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>5</v>
       </c>
       <c r="L18" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="S18" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="T18" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="U18" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="V18" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="W18" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="O18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="R18" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="T18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="U18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="V18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="W18" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="X18" s="1">
         <v>7</v>
       </c>
       <c r="Y18" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="Z18" s="6">
         <v>38965</v>
@@ -2589,13 +2591,13 @@
         <v>1</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="G19" s="5">
         <v>38174</v>
@@ -2604,55 +2606,55 @@
         <v>79990006</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="M19" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="T19" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="U19" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="V19" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="W19" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="O19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="R19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="S19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="T19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="U19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="V19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="W19" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="X19" s="1">
         <v>7</v>
       </c>
       <c r="Y19" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="Z19" s="6">
         <v>38966</v>
@@ -2674,10 +2676,10 @@
         <v>1</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="5">
@@ -2687,55 +2689,55 @@
         <v>79990007</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>5</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="N20" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="R20" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="S20" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="T20" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="U20" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="V20" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="W20" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="O20" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P20" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q20" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="R20" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="S20" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="T20" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="U20" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="V20" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="W20" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="X20" s="1">
         <v>7</v>
       </c>
       <c r="Y20" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="Z20" s="6">
         <v>38967</v>
@@ -2757,10 +2759,10 @@
         <v>1</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="5">
@@ -2770,55 +2772,55 @@
         <v>79990008</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>5</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="N21" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="T21" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="U21" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="V21" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="W21" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="O21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="R21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="S21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="T21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="U21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="V21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="W21" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="X21" s="1">
         <v>7</v>
       </c>
       <c r="Y21" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="Z21" s="6">
         <v>38968</v>
@@ -2840,10 +2842,10 @@
         <v>1</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="5">
@@ -2853,55 +2855,55 @@
         <v>79990009</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>5</v>
       </c>
       <c r="L22" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="S22" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="T22" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="U22" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="V22" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="W22" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="M22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="N22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="O22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="R22" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="T22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="U22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="V22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="W22" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="X22" s="1">
         <v>7</v>
       </c>
       <c r="Y22" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="Z22" s="6">
         <v>38969</v>
@@ -2923,13 +2925,13 @@
         <v>1</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="G23" s="5">
         <v>38178</v>
@@ -2938,55 +2940,55 @@
         <v>79990010</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="M23" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q23" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="R23" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="S23" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="T23" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="U23" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="V23" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="W23" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="N23" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="O23" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P23" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q23" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="R23" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="S23" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="T23" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="U23" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="V23" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="W23" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="X23" s="1">
         <v>7</v>
       </c>
       <c r="Y23" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="Z23" s="6">
         <v>38970</v>
@@ -3008,10 +3010,10 @@
         <v>1</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="5">
@@ -3021,55 +3023,55 @@
         <v>79990011</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>5</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="N24" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q24" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="R24" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="S24" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="T24" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="U24" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="V24" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="W24" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="O24" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P24" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q24" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="R24" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="S24" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="T24" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="U24" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="V24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="W24" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="X24" s="1">
         <v>7</v>
       </c>
       <c r="Y24" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="Z24" s="6">
         <v>38971</v>
@@ -3091,10 +3093,10 @@
         <v>1</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="5">
@@ -3104,55 +3106,55 @@
         <v>79990012</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>5</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="N25" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="R25" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="S25" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="T25" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="U25" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="V25" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="W25" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="O25" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P25" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q25" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="R25" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="S25" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="T25" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="U25" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="V25" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="W25" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="X25" s="1">
         <v>7</v>
       </c>
       <c r="Y25" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="Z25" s="6">
         <v>38972</v>
@@ -3174,13 +3176,13 @@
         <v>1</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="G26" s="5">
         <v>35735</v>
@@ -3189,7 +3191,7 @@
         <v>119990001</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="J26" s="3">
         <v>11</v>
@@ -3198,46 +3200,46 @@
         <v>5</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="N26" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q26" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="R26" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="S26" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="T26" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="U26" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="V26" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="W26" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="O26" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P26" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q26" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="R26" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="S26" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="T26" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="U26" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="V26" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="W26" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="X26" s="1">
         <v>11</v>
       </c>
       <c r="Y26" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="Z26" s="6">
         <v>37865</v>
@@ -3259,10 +3261,10 @@
         <v>1</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="5">
@@ -3272,55 +3274,55 @@
         <v>119990002</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="J27" s="3">
         <v>11</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="N27" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q27" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="R27" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="S27" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="T27" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="U27" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="V27" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="W27" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="O27" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P27" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q27" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="R27" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="S27" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="T27" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="U27" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="V27" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="W27" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="X27" s="1">
         <v>11</v>
       </c>
       <c r="Y27" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="Z27" s="6">
         <v>37866</v>
@@ -3342,10 +3344,10 @@
         <v>1</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="5">
@@ -3355,7 +3357,7 @@
         <v>119990003</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="J28" s="3">
         <v>11</v>
@@ -3364,46 +3366,46 @@
         <v>5</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="N28" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q28" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="R28" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="S28" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="T28" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="U28" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="V28" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="W28" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="O28" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P28" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q28" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="R28" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="S28" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="T28" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="U28" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="V28" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="W28" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="X28" s="1">
         <v>11</v>
       </c>
       <c r="Y28" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="Z28" s="6">
         <v>37867</v>
@@ -3425,10 +3427,10 @@
         <v>1</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="5">
@@ -3438,55 +3440,55 @@
         <v>119990004</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="J29" s="3">
         <v>11</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="Q29" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="R29" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="S29" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="T29" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="U29" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="V29" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="W29" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="R29" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="S29" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="T29" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="U29" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="V29" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="W29" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="X29" s="1">
         <v>11</v>
       </c>
       <c r="Y29" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="Z29" s="6">
         <v>37868</v>
@@ -3508,13 +3510,13 @@
         <v>1</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="G30" s="5">
         <v>35739</v>
@@ -3523,55 +3525,55 @@
         <v>119990005</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="J30" s="3">
         <v>11</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="N30" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="O30" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="P30" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q30" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="R30" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="S30" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="T30" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="U30" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="V30" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="W30" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="O30" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P30" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q30" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="R30" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="S30" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="T30" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="U30" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="V30" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="W30" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="X30" s="1">
         <v>11</v>
       </c>
       <c r="Y30" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="Z30" s="6">
         <v>37869</v>
@@ -3593,10 +3595,10 @@
         <v>1</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="5">
@@ -3606,7 +3608,7 @@
         <v>119990006</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="J31" s="3">
         <v>11</v>
@@ -3615,46 +3617,46 @@
         <v>5</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="N31" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="P31" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q31" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="R31" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="S31" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="T31" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="U31" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="V31" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="W31" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="O31" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P31" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q31" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="R31" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="S31" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="T31" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="U31" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="V31" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="W31" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="X31" s="1">
         <v>11</v>
       </c>
       <c r="Y31" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="Z31" s="6">
         <v>37870</v>
@@ -3676,10 +3678,10 @@
         <v>1</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="5">
@@ -3689,7 +3691,7 @@
         <v>119990007</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="J32" s="3">
         <v>11</v>
@@ -3698,46 +3700,46 @@
         <v>5</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="N32" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="P32" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q32" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="R32" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="S32" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="T32" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="U32" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="V32" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="W32" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="O32" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P32" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q32" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="R32" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="S32" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="T32" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="U32" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="V32" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="W32" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="X32" s="1">
         <v>11</v>
       </c>
       <c r="Y32" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="Z32" s="6">
         <v>37871</v>
@@ -3759,10 +3761,10 @@
         <v>1</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="5">
@@ -3772,55 +3774,55 @@
         <v>119990008</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="J33" s="3">
         <v>11</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="Q33" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="R33" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="S33" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="T33" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="U33" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="V33" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="W33" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="R33" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="S33" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="T33" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="U33" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="V33" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="W33" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="X33" s="1">
         <v>11</v>
       </c>
       <c r="Y33" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="Z33" s="6">
         <v>37872</v>
@@ -3842,13 +3844,13 @@
         <v>1</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="G34" s="5">
         <v>35743</v>
@@ -3857,7 +3859,7 @@
         <v>119990009</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="J34" s="3">
         <v>11</v>
@@ -3866,46 +3868,46 @@
         <v>5</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="N34" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="O34" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="P34" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q34" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="R34" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="S34" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="T34" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="U34" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="V34" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="W34" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="O34" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P34" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q34" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="R34" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="S34" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="T34" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="U34" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="V34" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="W34" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="X34" s="1">
         <v>11</v>
       </c>
       <c r="Y34" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="Z34" s="6">
         <v>37873</v>
@@ -3927,10 +3929,10 @@
         <v>1</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="F35" s="1"/>
       <c r="G35" s="5">
@@ -3940,55 +3942,55 @@
         <v>119990010</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="J35" s="3">
         <v>11</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="N35" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="O35" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="P35" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q35" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="R35" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="S35" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="T35" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="U35" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="V35" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="W35" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="O35" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P35" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q35" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="R35" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="S35" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="T35" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="U35" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="V35" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="W35" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="X35" s="1">
         <v>11</v>
       </c>
       <c r="Y35" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="Z35" s="6">
         <v>37874</v>
@@ -4010,10 +4012,10 @@
         <v>1</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="5">
@@ -4023,7 +4025,7 @@
         <v>119990011</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="J36" s="3">
         <v>11</v>
@@ -4032,46 +4034,46 @@
         <v>5</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="N36" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="O36" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="P36" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q36" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="R36" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="S36" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="T36" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="U36" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="V36" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="W36" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="O36" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P36" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q36" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="R36" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="S36" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="T36" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="U36" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="V36" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="W36" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="X36" s="1">
         <v>11</v>
       </c>
       <c r="Y36" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="Z36" s="6">
         <v>37875</v>
@@ -4093,10 +4095,10 @@
         <v>1</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="5">
@@ -4106,55 +4108,55 @@
         <v>119990012</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="J37" s="3">
         <v>11</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="Q37" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="R37" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="S37" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="T37" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="U37" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="V37" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="W37" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="R37" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="S37" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="T37" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="U37" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="V37" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="W37" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="X37" s="1">
         <v>11</v>
       </c>
       <c r="Y37" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="Z37" s="6">
         <v>37876</v>

</xml_diff>

<commit_message>
Updated UI and PDF report so only four columns are shown: Status, Field, Expected Value, and Actual Value. An additional error row will follow any fields that contain an error. The error row will display the error.
</commit_message>
<xml_diff>
--- a/irp-webapp/src/main/resources/irp-package/IRPStudents.xlsx
+++ b/irp-webapp/src/main/resources/irp-package/IRPStudents.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="20" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="20" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="STUDENT" sheetId="1" r:id="rId1"/>
@@ -1032,15 +1032,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="AD1" sqref="AD1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="4"/>
     <col min="2" max="2" width="24.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="10.83203125" style="4"/>
+    <col min="3" max="3" width="27" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="9" width="10.83203125" style="4"/>
     <col min="10" max="10" width="10.83203125" style="2"/>
     <col min="11" max="22" width="10.83203125" style="4"/>
     <col min="23" max="23" width="13.1640625" style="4" bestFit="1" customWidth="1"/>

</xml_diff>